<commit_message>
fixed bug in entity identification function.
</commit_message>
<xml_diff>
--- a/kikar_hamedina/Alternative Names.xlsx
+++ b/kikar_hamedina/Alternative Names.xlsx
@@ -1875,9 +1875,6 @@
     <t>הנגבי;hanegbi;Tzachi Hanegbi;</t>
   </si>
   <si>
-    <t>בנימין;Benyamin;Benjamin</t>
-  </si>
-  <si>
     <t>יאיר;Yair;יאירקה;</t>
   </si>
   <si>
@@ -2410,6 +2407,9 @@
   </si>
   <si>
     <t>Hillel Horowitz;</t>
+  </si>
+  <si>
+    <t>בנימין;Benyamin;Benjamin;BB</t>
   </si>
 </sst>
 </file>
@@ -2761,8 +2761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2925,7 +2925,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F8" t="s">
         <v>363</v>
@@ -2965,7 +2965,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F10" t="s">
         <v>365</v>
@@ -3005,10 +3005,10 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
+        <v>632</v>
+      </c>
+      <c r="E12" t="s">
         <v>633</v>
-      </c>
-      <c r="E12" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -3022,13 +3022,13 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
+        <v>636</v>
+      </c>
+      <c r="E13" t="s">
+        <v>787</v>
+      </c>
+      <c r="F13" t="s">
         <v>637</v>
-      </c>
-      <c r="E13" t="s">
-        <v>609</v>
-      </c>
-      <c r="F13" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3062,7 +3062,7 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H15" t="s">
         <v>356</v>
@@ -3096,7 +3096,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -4062,7 +4062,7 @@
         <v>505</v>
       </c>
       <c r="E71" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4525,10 +4525,10 @@
         <v>69</v>
       </c>
       <c r="D97" t="s">
+        <v>628</v>
+      </c>
+      <c r="E97" t="s">
         <v>629</v>
-      </c>
-      <c r="E97" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -4596,7 +4596,7 @@
         <v>69</v>
       </c>
       <c r="D101" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H101" t="s">
         <v>356</v>
@@ -4985,10 +4985,10 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E123" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -5002,10 +5002,10 @@
         <v>112</v>
       </c>
       <c r="D124" t="s">
+        <v>612</v>
+      </c>
+      <c r="E124" t="s">
         <v>613</v>
-      </c>
-      <c r="E124" t="s">
-        <v>614</v>
       </c>
       <c r="F124" t="s">
         <v>393</v>
@@ -5022,10 +5022,10 @@
         <v>69</v>
       </c>
       <c r="D125" t="s">
+        <v>625</v>
+      </c>
+      <c r="E125" t="s">
         <v>626</v>
-      </c>
-      <c r="E125" t="s">
-        <v>627</v>
       </c>
       <c r="F125" t="s">
         <v>394</v>
@@ -5042,10 +5042,10 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E126" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -5059,10 +5059,10 @@
         <v>41</v>
       </c>
       <c r="D127" t="s">
+        <v>616</v>
+      </c>
+      <c r="E127" t="s">
         <v>617</v>
-      </c>
-      <c r="E127" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -5076,10 +5076,10 @@
         <v>35</v>
       </c>
       <c r="D128" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E128" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -5093,10 +5093,10 @@
         <v>6</v>
       </c>
       <c r="D129" t="s">
+        <v>620</v>
+      </c>
+      <c r="E129" t="s">
         <v>621</v>
-      </c>
-      <c r="E129" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -5110,7 +5110,7 @@
         <v>18</v>
       </c>
       <c r="D130" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G130" t="s">
         <v>356</v>
@@ -5127,10 +5127,10 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
+        <v>623</v>
+      </c>
+      <c r="E131" t="s">
         <v>624</v>
-      </c>
-      <c r="E131" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -5138,16 +5138,16 @@
         <v>20</v>
       </c>
       <c r="B132" t="s">
+        <v>638</v>
+      </c>
+      <c r="C132" t="s">
         <v>639</v>
       </c>
-      <c r="C132" t="s">
-        <v>640</v>
-      </c>
       <c r="D132" t="s">
+        <v>694</v>
+      </c>
+      <c r="E132" t="s">
         <v>695</v>
-      </c>
-      <c r="E132" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -5155,16 +5155,16 @@
         <v>63</v>
       </c>
       <c r="B133" t="s">
+        <v>640</v>
+      </c>
+      <c r="C133" t="s">
         <v>641</v>
       </c>
-      <c r="C133" t="s">
-        <v>642</v>
-      </c>
       <c r="D133" t="s">
+        <v>696</v>
+      </c>
+      <c r="E133" t="s">
         <v>697</v>
-      </c>
-      <c r="E133" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -5172,16 +5172,16 @@
         <v>70</v>
       </c>
       <c r="B134" t="s">
+        <v>642</v>
+      </c>
+      <c r="C134" t="s">
         <v>643</v>
       </c>
-      <c r="C134" t="s">
-        <v>644</v>
-      </c>
       <c r="D134" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E134" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -5189,16 +5189,16 @@
         <v>77</v>
       </c>
       <c r="B135" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C135" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D135" t="s">
+        <v>700</v>
+      </c>
+      <c r="E135" t="s">
         <v>701</v>
-      </c>
-      <c r="E135" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -5206,16 +5206,16 @@
         <v>114</v>
       </c>
       <c r="B136" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C136" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D136" t="s">
+        <v>702</v>
+      </c>
+      <c r="E136" t="s">
         <v>703</v>
-      </c>
-      <c r="E136" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -5223,16 +5223,16 @@
         <v>119</v>
       </c>
       <c r="B137" t="s">
+        <v>646</v>
+      </c>
+      <c r="C137" t="s">
         <v>647</v>
       </c>
-      <c r="C137" t="s">
-        <v>648</v>
-      </c>
       <c r="D137" t="s">
+        <v>704</v>
+      </c>
+      <c r="E137" t="s">
         <v>705</v>
-      </c>
-      <c r="E137" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -5240,16 +5240,16 @@
         <v>197</v>
       </c>
       <c r="B138" t="s">
+        <v>648</v>
+      </c>
+      <c r="C138" t="s">
         <v>649</v>
       </c>
-      <c r="C138" t="s">
-        <v>650</v>
-      </c>
       <c r="D138" t="s">
+        <v>706</v>
+      </c>
+      <c r="E138" t="s">
         <v>707</v>
-      </c>
-      <c r="E138" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -5257,13 +5257,13 @@
         <v>206</v>
       </c>
       <c r="B139" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C139" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D139" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G139" t="s">
         <v>356</v>
@@ -5274,13 +5274,13 @@
         <v>210</v>
       </c>
       <c r="B140" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C140" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D140" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G140" t="s">
         <v>356</v>
@@ -5291,16 +5291,16 @@
         <v>720</v>
       </c>
       <c r="B141" t="s">
+        <v>652</v>
+      </c>
+      <c r="C141" t="s">
         <v>653</v>
       </c>
-      <c r="C141" t="s">
-        <v>654</v>
-      </c>
       <c r="D141" t="s">
+        <v>710</v>
+      </c>
+      <c r="E141" t="s">
         <v>711</v>
-      </c>
-      <c r="E141" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -5308,16 +5308,16 @@
         <v>725</v>
       </c>
       <c r="B142" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C142" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D142" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E142" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -5325,16 +5325,16 @@
         <v>739</v>
       </c>
       <c r="B143" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C143" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D143" t="s">
+        <v>714</v>
+      </c>
+      <c r="E143" t="s">
         <v>715</v>
-      </c>
-      <c r="E143" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -5342,16 +5342,16 @@
         <v>758</v>
       </c>
       <c r="B144" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C144" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D144" t="s">
+        <v>716</v>
+      </c>
+      <c r="E144" t="s">
         <v>717</v>
-      </c>
-      <c r="E144" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -5359,16 +5359,16 @@
         <v>781</v>
       </c>
       <c r="B145" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C145" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D145" t="s">
+        <v>718</v>
+      </c>
+      <c r="E145" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -5376,13 +5376,13 @@
         <v>784</v>
       </c>
       <c r="B146" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C146" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D146" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G146" t="s">
         <v>356</v>
@@ -5393,16 +5393,16 @@
         <v>785</v>
       </c>
       <c r="B147" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C147" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D147" t="s">
+        <v>721</v>
+      </c>
+      <c r="E147" t="s">
         <v>722</v>
-      </c>
-      <c r="E147" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -5410,16 +5410,16 @@
         <v>789</v>
       </c>
       <c r="B148" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C148" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D148" t="s">
+        <v>723</v>
+      </c>
+      <c r="E148" t="s">
         <v>724</v>
-      </c>
-      <c r="E148" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -5427,16 +5427,16 @@
         <v>790</v>
       </c>
       <c r="B149" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C149" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D149" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E149" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -5444,16 +5444,16 @@
         <v>791</v>
       </c>
       <c r="B150" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C150" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D150" t="s">
+        <v>727</v>
+      </c>
+      <c r="E150" t="s">
         <v>728</v>
-      </c>
-      <c r="E150" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -5461,16 +5461,16 @@
         <v>797</v>
       </c>
       <c r="B151" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C151" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D151" t="s">
+        <v>729</v>
+      </c>
+      <c r="E151" t="s">
         <v>730</v>
-      </c>
-      <c r="E151" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -5478,16 +5478,16 @@
         <v>800</v>
       </c>
       <c r="B152" t="s">
+        <v>664</v>
+      </c>
+      <c r="C152" t="s">
         <v>665</v>
       </c>
-      <c r="C152" t="s">
-        <v>666</v>
-      </c>
       <c r="D152" t="s">
+        <v>731</v>
+      </c>
+      <c r="E152" t="s">
         <v>732</v>
-      </c>
-      <c r="E152" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -5495,16 +5495,16 @@
         <v>805</v>
       </c>
       <c r="B153" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C153" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D153" t="s">
+        <v>733</v>
+      </c>
+      <c r="E153" t="s">
         <v>734</v>
-      </c>
-      <c r="E153" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -5512,16 +5512,16 @@
         <v>813</v>
       </c>
       <c r="B154" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C154" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D154" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E154" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -5529,16 +5529,16 @@
         <v>829</v>
       </c>
       <c r="B155" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C155" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D155" t="s">
+        <v>737</v>
+      </c>
+      <c r="E155" t="s">
         <v>738</v>
-      </c>
-      <c r="E155" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -5546,16 +5546,16 @@
         <v>835</v>
       </c>
       <c r="B156" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C156" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D156" t="s">
+        <v>739</v>
+      </c>
+      <c r="E156" t="s">
         <v>740</v>
-      </c>
-      <c r="E156" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -5563,16 +5563,16 @@
         <v>842</v>
       </c>
       <c r="B157" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C157" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D157" t="s">
+        <v>741</v>
+      </c>
+      <c r="E157" t="s">
         <v>742</v>
-      </c>
-      <c r="E157" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -5580,16 +5580,16 @@
         <v>843</v>
       </c>
       <c r="B158" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C158" t="s">
         <v>63</v>
       </c>
       <c r="D158" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E158" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5597,16 +5597,16 @@
         <v>845</v>
       </c>
       <c r="B159" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C159" t="s">
         <v>53</v>
       </c>
       <c r="D159" t="s">
+        <v>745</v>
+      </c>
+      <c r="E159" t="s">
         <v>746</v>
-      </c>
-      <c r="E159" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -5614,16 +5614,16 @@
         <v>853</v>
       </c>
       <c r="B160" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C160" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D160" t="s">
+        <v>747</v>
+      </c>
+      <c r="E160" t="s">
         <v>748</v>
-      </c>
-      <c r="E160" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5631,16 +5631,16 @@
         <v>859</v>
       </c>
       <c r="B161" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C161" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D161" t="s">
+        <v>749</v>
+      </c>
+      <c r="E161" t="s">
         <v>750</v>
-      </c>
-      <c r="E161" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5648,13 +5648,13 @@
         <v>861</v>
       </c>
       <c r="B162" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C162" t="s">
         <v>23</v>
       </c>
       <c r="D162" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G162" t="s">
         <v>356</v>
@@ -5665,16 +5665,16 @@
         <v>869</v>
       </c>
       <c r="B163" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C163" t="s">
         <v>197</v>
       </c>
       <c r="D163" t="s">
+        <v>752</v>
+      </c>
+      <c r="E163" t="s">
         <v>753</v>
-      </c>
-      <c r="E163" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5682,16 +5682,16 @@
         <v>872</v>
       </c>
       <c r="B164" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C164" t="s">
         <v>197</v>
       </c>
       <c r="D164" t="s">
+        <v>754</v>
+      </c>
+      <c r="E164" t="s">
         <v>755</v>
-      </c>
-      <c r="E164" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5699,16 +5699,16 @@
         <v>877</v>
       </c>
       <c r="B165" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C165" t="s">
         <v>197</v>
       </c>
       <c r="D165" t="s">
+        <v>756</v>
+      </c>
+      <c r="E165" t="s">
         <v>757</v>
-      </c>
-      <c r="E165" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5716,16 +5716,16 @@
         <v>880</v>
       </c>
       <c r="B166" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C166" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D166" t="s">
+        <v>758</v>
+      </c>
+      <c r="E166" t="s">
         <v>759</v>
-      </c>
-      <c r="E166" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5733,16 +5733,16 @@
         <v>883</v>
       </c>
       <c r="B167" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C167" t="s">
         <v>197</v>
       </c>
       <c r="D167" t="s">
+        <v>760</v>
+      </c>
+      <c r="E167" t="s">
         <v>761</v>
-      </c>
-      <c r="E167" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5750,16 +5750,16 @@
         <v>884</v>
       </c>
       <c r="B168" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C168" t="s">
         <v>53</v>
       </c>
       <c r="D168" t="s">
+        <v>762</v>
+      </c>
+      <c r="E168" t="s">
         <v>763</v>
-      </c>
-      <c r="E168" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5767,16 +5767,16 @@
         <v>885</v>
       </c>
       <c r="B169" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C169" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D169" t="s">
+        <v>764</v>
+      </c>
+      <c r="E169" t="s">
         <v>765</v>
-      </c>
-      <c r="E169" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5784,16 +5784,16 @@
         <v>889</v>
       </c>
       <c r="B170" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C170" t="s">
         <v>197</v>
       </c>
       <c r="D170" t="s">
+        <v>766</v>
+      </c>
+      <c r="E170" t="s">
         <v>767</v>
-      </c>
-      <c r="E170" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5801,16 +5801,16 @@
         <v>890</v>
       </c>
       <c r="B171" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C171" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D171" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E171" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5818,16 +5818,16 @@
         <v>891</v>
       </c>
       <c r="B172" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C172" t="s">
         <v>197</v>
       </c>
       <c r="D172" t="s">
+        <v>770</v>
+      </c>
+      <c r="E172" t="s">
         <v>771</v>
-      </c>
-      <c r="E172" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5835,16 +5835,16 @@
         <v>892</v>
       </c>
       <c r="B173" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C173" t="s">
         <v>197</v>
       </c>
       <c r="D173" t="s">
+        <v>772</v>
+      </c>
+      <c r="E173" t="s">
         <v>773</v>
-      </c>
-      <c r="E173" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5852,16 +5852,16 @@
         <v>893</v>
       </c>
       <c r="B174" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C174" t="s">
         <v>53</v>
       </c>
       <c r="D174" t="s">
+        <v>774</v>
+      </c>
+      <c r="E174" t="s">
         <v>775</v>
-      </c>
-      <c r="E174" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5869,16 +5869,16 @@
         <v>894</v>
       </c>
       <c r="B175" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C175" t="s">
         <v>197</v>
       </c>
       <c r="D175" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E175" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5886,16 +5886,16 @@
         <v>898</v>
       </c>
       <c r="B176" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C176" t="s">
         <v>53</v>
       </c>
       <c r="D176" t="s">
+        <v>778</v>
+      </c>
+      <c r="E176" t="s">
         <v>779</v>
-      </c>
-      <c r="E176" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5903,16 +5903,16 @@
         <v>902</v>
       </c>
       <c r="B177" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C177" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D177" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E177" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -5920,16 +5920,16 @@
         <v>905</v>
       </c>
       <c r="B178" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C178" t="s">
         <v>197</v>
       </c>
       <c r="D178" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E178" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -5937,16 +5937,16 @@
         <v>907</v>
       </c>
       <c r="B179" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C179" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D179" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G179" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -5954,13 +5954,13 @@
         <v>908</v>
       </c>
       <c r="B180" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C180" t="s">
         <v>53</v>
       </c>
       <c r="D180" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -13040,10 +13040,10 @@
         <v>20</v>
       </c>
       <c r="B133" t="s">
+        <v>638</v>
+      </c>
+      <c r="C133" t="s">
         <v>639</v>
-      </c>
-      <c r="C133" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -13051,10 +13051,10 @@
         <v>63</v>
       </c>
       <c r="B134" t="s">
+        <v>640</v>
+      </c>
+      <c r="C134" t="s">
         <v>641</v>
-      </c>
-      <c r="C134" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -13062,10 +13062,10 @@
         <v>70</v>
       </c>
       <c r="B135" t="s">
+        <v>642</v>
+      </c>
+      <c r="C135" t="s">
         <v>643</v>
-      </c>
-      <c r="C135" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -13073,10 +13073,10 @@
         <v>77</v>
       </c>
       <c r="B136" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C136" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -13084,10 +13084,10 @@
         <v>114</v>
       </c>
       <c r="B137" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C137" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -13095,10 +13095,10 @@
         <v>119</v>
       </c>
       <c r="B138" t="s">
+        <v>646</v>
+      </c>
+      <c r="C138" t="s">
         <v>647</v>
-      </c>
-      <c r="C138" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -13106,10 +13106,10 @@
         <v>197</v>
       </c>
       <c r="B139" t="s">
+        <v>648</v>
+      </c>
+      <c r="C139" t="s">
         <v>649</v>
-      </c>
-      <c r="C139" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -13117,10 +13117,10 @@
         <v>206</v>
       </c>
       <c r="B140" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C140" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -13128,10 +13128,10 @@
         <v>210</v>
       </c>
       <c r="B141" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C141" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -13139,10 +13139,10 @@
         <v>720</v>
       </c>
       <c r="B142" t="s">
+        <v>652</v>
+      </c>
+      <c r="C142" t="s">
         <v>653</v>
-      </c>
-      <c r="C142" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -13150,10 +13150,10 @@
         <v>725</v>
       </c>
       <c r="B143" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C143" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -13161,10 +13161,10 @@
         <v>739</v>
       </c>
       <c r="B144" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C144" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -13172,10 +13172,10 @@
         <v>758</v>
       </c>
       <c r="B145" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C145" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -13183,10 +13183,10 @@
         <v>781</v>
       </c>
       <c r="B146" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C146" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -13194,10 +13194,10 @@
         <v>784</v>
       </c>
       <c r="B147" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C147" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -13205,10 +13205,10 @@
         <v>785</v>
       </c>
       <c r="B148" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C148" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -13216,10 +13216,10 @@
         <v>789</v>
       </c>
       <c r="B149" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C149" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -13227,10 +13227,10 @@
         <v>790</v>
       </c>
       <c r="B150" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C150" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -13238,10 +13238,10 @@
         <v>791</v>
       </c>
       <c r="B151" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C151" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -13249,10 +13249,10 @@
         <v>797</v>
       </c>
       <c r="B152" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C152" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -13260,10 +13260,10 @@
         <v>800</v>
       </c>
       <c r="B153" t="s">
+        <v>664</v>
+      </c>
+      <c r="C153" t="s">
         <v>665</v>
-      </c>
-      <c r="C153" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -13271,10 +13271,10 @@
         <v>805</v>
       </c>
       <c r="B154" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C154" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -13282,10 +13282,10 @@
         <v>813</v>
       </c>
       <c r="B155" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C155" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -13293,10 +13293,10 @@
         <v>829</v>
       </c>
       <c r="B156" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C156" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -13304,10 +13304,10 @@
         <v>835</v>
       </c>
       <c r="B157" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C157" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -13315,10 +13315,10 @@
         <v>842</v>
       </c>
       <c r="B158" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C158" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -13326,7 +13326,7 @@
         <v>843</v>
       </c>
       <c r="B159" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C159" t="s">
         <v>63</v>
@@ -13337,7 +13337,7 @@
         <v>845</v>
       </c>
       <c r="B160" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C160" t="s">
         <v>53</v>
@@ -13348,10 +13348,10 @@
         <v>853</v>
       </c>
       <c r="B161" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C161" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -13359,10 +13359,10 @@
         <v>859</v>
       </c>
       <c r="B162" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C162" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -13370,7 +13370,7 @@
         <v>861</v>
       </c>
       <c r="B163" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C163" t="s">
         <v>23</v>
@@ -13381,7 +13381,7 @@
         <v>869</v>
       </c>
       <c r="B164" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C164" t="s">
         <v>197</v>
@@ -13392,7 +13392,7 @@
         <v>872</v>
       </c>
       <c r="B165" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C165" t="s">
         <v>197</v>
@@ -13403,7 +13403,7 @@
         <v>877</v>
       </c>
       <c r="B166" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C166" t="s">
         <v>197</v>
@@ -13414,10 +13414,10 @@
         <v>880</v>
       </c>
       <c r="B167" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C167" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -13425,7 +13425,7 @@
         <v>883</v>
       </c>
       <c r="B168" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C168" t="s">
         <v>197</v>
@@ -13436,7 +13436,7 @@
         <v>884</v>
       </c>
       <c r="B169" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C169" t="s">
         <v>53</v>
@@ -13447,10 +13447,10 @@
         <v>885</v>
       </c>
       <c r="B170" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C170" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -13458,7 +13458,7 @@
         <v>889</v>
       </c>
       <c r="B171" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C171" t="s">
         <v>197</v>
@@ -13469,10 +13469,10 @@
         <v>890</v>
       </c>
       <c r="B172" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C172" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -13480,7 +13480,7 @@
         <v>891</v>
       </c>
       <c r="B173" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C173" t="s">
         <v>197</v>
@@ -13491,7 +13491,7 @@
         <v>892</v>
       </c>
       <c r="B174" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C174" t="s">
         <v>197</v>
@@ -13502,7 +13502,7 @@
         <v>893</v>
       </c>
       <c r="B175" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C175" t="s">
         <v>53</v>
@@ -13513,7 +13513,7 @@
         <v>894</v>
       </c>
       <c r="B176" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C176" t="s">
         <v>197</v>
@@ -13524,7 +13524,7 @@
         <v>898</v>
       </c>
       <c r="B177" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C177" t="s">
         <v>53</v>
@@ -13535,10 +13535,10 @@
         <v>902</v>
       </c>
       <c r="B178" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C178" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -13546,7 +13546,7 @@
         <v>905</v>
       </c>
       <c r="B179" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C179" t="s">
         <v>197</v>
@@ -13557,10 +13557,10 @@
         <v>907</v>
       </c>
       <c r="B180" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C180" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -13568,7 +13568,7 @@
         <v>908</v>
       </c>
       <c r="B181" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C181" t="s">
         <v>53</v>

</xml_diff>